<commit_message>
fixed job title issue
</commit_message>
<xml_diff>
--- a/DailyHotList.xlsx
+++ b/DailyHotList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somep\OneDrive\Documents\Automation\SendHotlistMails-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somep\OneDrive\Documents\Automation\Seafysoft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEC588-CA01-4D34-9332-47268391B8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368B4CFE-0D3A-44C5-BEA7-069D2F33B603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{034D8F17-0AC6-E54A-9B60-385E6FDBED45}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{034D8F17-0AC6-E54A-9B60-385E6FDBED45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Experience</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Oracle HCM,Oracle,Oracle Fusion,Oracle Cloud,Oracle Apps</t>
+  </si>
+  <si>
+    <t>JobTitle</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A358D4-0865-C549-BC3A-BE2133E80F40}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -654,211 +654,211 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C945F027-FA8B-482B-ADBB-D495D94C6CE1}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -881,106 +881,106 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1007,97 +1007,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>